<commit_message>
Dienstag morgen - Gini fern tests done.
</commit_message>
<xml_diff>
--- a/Code/Ferns/Heuristical Ferns/Evaluation/Times_Gini_Random.xlsx
+++ b/Code/Ferns/Heuristical Ferns/Evaluation/Times_Gini_Random.xlsx
@@ -95,7 +95,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -252,11 +252,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63867520"/>
-        <c:axId val="63881600"/>
+        <c:axId val="74461696"/>
+        <c:axId val="97190464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63867520"/>
+        <c:axId val="74461696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -266,7 +266,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63881600"/>
+        <c:crossAx val="97190464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -274,7 +274,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63881600"/>
+        <c:axId val="97190464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -285,7 +285,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63867520"/>
+        <c:crossAx val="74461696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -311,16 +311,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,25 +796,43 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="E12" s="1">
+        <v>14.3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1343.6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>5</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="E13" s="1">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6344.4</v>
+      </c>
+      <c r="G13" s="1">
+        <v>67.8</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>10</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="E14" s="1">
+        <v>205</v>
+      </c>
+      <c r="F14" s="1">
+        <v>12917</v>
+      </c>
+      <c r="G14" s="1">
+        <v>115</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C15">
@@ -855,25 +873,43 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="E19" s="1">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1">
+        <v>501</v>
+      </c>
+      <c r="G19" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>5</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="E20" s="1">
+        <v>95</v>
+      </c>
+      <c r="F20" s="1">
+        <v>9129</v>
+      </c>
+      <c r="G20" s="1">
+        <v>71</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>10</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="E21" s="1">
+        <v>164</v>
+      </c>
+      <c r="F21" s="1">
+        <v>10048</v>
+      </c>
+      <c r="G21" s="1">
+        <v>113</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22">

</xml_diff>